<commit_message>
lots of organisation documents
</commit_message>
<xml_diff>
--- a/Org/Semester 2/Sprint_1.xlsx
+++ b/Org/Semester 2/Sprint_1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\OneDrive\Studium\FHTechnikum\3. Semester\9_InnoLab\LocalRep\Org\Semester 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee58e90f1ffcc7c2/Studium/FHTechnikum/3. Semester/9_InnoLab/LocalRep/Org/Semester 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_01DF930F10C4914B2615C79761E3592926E9BEC3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98802427-EA7F-4FC7-8429-FC344EC7A6C6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="13200"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$I$27</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +29,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -151,7 +155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,7 +423,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -436,11 +440,32 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -457,12 +482,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -487,44 +506,44 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="4"/>
-    <cellStyle name="Normal 5" xfId="5"/>
-    <cellStyle name="Normal 7" xfId="6"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 5" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 7" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 10" xfId="1"/>
-    <cellStyle name="Standard 2" xfId="2"/>
-    <cellStyle name="Standard 2 2" xfId="7"/>
-    <cellStyle name="Standard 3" xfId="14"/>
-    <cellStyle name="Standard 4" xfId="9"/>
-    <cellStyle name="Standard 5" xfId="8"/>
-    <cellStyle name="Standard 6" xfId="10"/>
-    <cellStyle name="Standard 7" xfId="11"/>
-    <cellStyle name="Standard 8" xfId="12"/>
-    <cellStyle name="Standard 9" xfId="13"/>
+    <cellStyle name="Standard 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Standard 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Standard 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Standard 3" xfId="14" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Standard 4" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Standard 5" xfId="8" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Standard 6" xfId="10" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Standard 7" xfId="11" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Standard 8" xfId="12" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Standard 9" xfId="13" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -835,11 +854,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -856,28 +875,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -891,131 +910,131 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="19">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
         <v>1</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="21">
+      <c r="B5" s="13"/>
+      <c r="C5" s="26">
         <v>45741.71875</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="23">
+      <c r="B6" s="13"/>
+      <c r="C6" s="28">
         <v>16</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="24"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="25" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="31"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="27" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1044,180 +1063,180 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="38">
         <v>1</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="32">
         <v>15</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="32">
         <v>8</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="34">
         <f>D16-C16</f>
         <v>-7</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="32"/>
     </row>
     <row r="17" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="A17" s="38">
         <v>2</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="32">
         <v>10</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="32">
         <v>7</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="34">
         <f t="shared" ref="E17:E25" si="0">D17-C17</f>
         <v>-3</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="7"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="A18" s="38">
         <v>3</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="32">
         <v>10</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="32">
         <v>8</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="34">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="7"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="38">
         <v>4</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="32">
         <v>15</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="32">
         <v>22</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="34">
         <f>D19-C19</f>
         <v>7</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="7"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="32"/>
     </row>
     <row r="20" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="38">
         <v>5</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="32">
         <v>18</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="32">
         <v>20</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="34">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="7"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="32"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="38">
         <v>6</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="32">
         <v>10</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="32">
         <v>9</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="34">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="7"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="32"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="38">
         <v>7</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="32">
         <v>35</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="32">
         <v>33</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="34">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="7"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="32"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="2">
+      <c r="B23" s="33"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="7"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="32"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
@@ -1297,12 +1316,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C11:G11"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -1317,6 +1330,12 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C11:G11"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="87" orientation="landscape" r:id="rId1"/>

</xml_diff>